<commit_message>
New plots and latest data
</commit_message>
<xml_diff>
--- a/Picobirnavirus Summary.xlsx
+++ b/Picobirnavirus Summary.xlsx
@@ -18,9 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="173">
   <si>
-    <t>Protien</t>
-  </si>
-  <si>
     <t>Nucleotide</t>
   </si>
   <si>
@@ -535,6 +532,9 @@
   </si>
   <si>
     <t>38</t>
+  </si>
+  <si>
+    <t>Protein</t>
   </si>
 </sst>
 </file>
@@ -915,7 +915,7 @@
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,1373 +934,1373 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" t="s">
-        <v>33</v>
-      </c>
       <c r="J1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="I2">
         <v>2009</v>
       </c>
       <c r="J2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K2">
         <v>2007</v>
       </c>
       <c r="L2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="I3">
         <v>2009</v>
       </c>
       <c r="J3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K3">
         <v>2007</v>
       </c>
       <c r="L3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="I4">
         <v>2009</v>
       </c>
       <c r="J4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K4">
         <v>2007</v>
       </c>
       <c r="L4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="I5">
         <v>2009</v>
       </c>
       <c r="J5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K5">
         <v>2007</v>
       </c>
       <c r="L5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>132</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" t="s">
-        <v>133</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="I6">
         <v>2009</v>
       </c>
       <c r="J6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K6">
         <v>2007</v>
       </c>
       <c r="L6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I7">
         <v>2013</v>
       </c>
       <c r="J7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K7">
         <v>2013</v>
       </c>
       <c r="L7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I8">
         <v>2000</v>
       </c>
       <c r="J8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I9">
         <v>2000</v>
       </c>
       <c r="J9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" t="s">
         <v>12</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="I10">
         <v>2009</v>
       </c>
       <c r="J10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K10">
         <v>2005</v>
       </c>
       <c r="L10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" t="s">
         <v>16</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I11">
         <v>2012</v>
       </c>
       <c r="J11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K11">
         <v>2008</v>
       </c>
       <c r="L11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="I12">
         <v>2013</v>
       </c>
       <c r="J12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K12">
         <v>2012</v>
       </c>
       <c r="L12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I13">
         <v>2013</v>
       </c>
       <c r="J13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K13">
         <v>2013</v>
       </c>
       <c r="L13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" t="s">
         <v>28</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="F14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="I14">
         <v>2013</v>
       </c>
       <c r="J14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K14">
         <v>2004</v>
       </c>
       <c r="L14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
         <v>64</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="H15" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="I15">
         <v>2014</v>
       </c>
       <c r="J15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K15">
         <v>2011</v>
       </c>
       <c r="L15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="F16" t="s">
-        <v>26</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="I16">
         <v>2014</v>
       </c>
       <c r="J16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K16">
         <v>2013</v>
       </c>
       <c r="L16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="F17" t="s">
-        <v>26</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="I17">
         <v>2014</v>
       </c>
       <c r="J17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K17">
         <v>2013</v>
       </c>
       <c r="L17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I18">
         <v>2014</v>
       </c>
       <c r="J18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K18">
         <v>2013</v>
       </c>
       <c r="L18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="F19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I19">
         <v>2014</v>
       </c>
       <c r="J19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K19">
         <v>2013</v>
       </c>
       <c r="L19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I20">
         <v>2014</v>
       </c>
       <c r="J20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K20">
         <v>2013</v>
       </c>
       <c r="L20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="D21" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I21">
         <v>2016</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K21">
         <v>2008</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="D22" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I22">
         <v>2016</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K22">
         <v>2008</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="D23" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I23">
         <v>2016</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K23">
         <v>2008</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="D24" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I24">
         <v>2016</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K24">
         <v>2008</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="D25" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I25">
         <v>2016</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K25">
         <v>2008</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="D26" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I26">
         <v>2016</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K26">
         <v>2008</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="D27" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I27">
         <v>2016</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K27">
         <v>2009</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="D28" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I28">
         <v>2016</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K28">
         <v>2009</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="D29" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I29">
         <v>2016</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K29">
         <v>2009</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I30">
         <v>2016</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K30">
         <v>2009</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="D31" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I31">
         <v>2016</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K31">
         <v>2009</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="D32" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I32">
         <v>2016</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K32">
         <v>2009</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I33">
         <v>2016</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K33">
         <v>2009</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B34" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="D34" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I34">
         <v>2016</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K34">
         <v>2010</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="E35" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I35">
         <v>2016</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K35">
         <v>2010</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I36">
         <v>2016</v>
       </c>
       <c r="J36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K36">
         <v>2014</v>
       </c>
       <c r="L36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="H37" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I37">
         <v>2016</v>
       </c>
       <c r="J37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K37">
         <v>2013</v>
       </c>
       <c r="L37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I38">
         <v>2016</v>
       </c>
       <c r="J38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K38">
         <v>2014</v>
       </c>
       <c r="L38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="I39">
         <v>2004</v>
       </c>
       <c r="J39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>